<commit_message>
update practice block fish color assignments
</commit_message>
<xml_diff>
--- a/html/resources/1condition/practiceTrials1.xlsx
+++ b/html/resources/1condition/practiceTrials1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janet/Desktop/Sinai_Projects/Code/fish-task-6B20T/html/resources/1condition/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janet/Documents/Sinai_Projects/Code/fish-task-6B20T/html/resources/1condition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412EA95F-3E63-A844-9476-62B8CE827246}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE34F045-6D28-844D-A5DF-B91A129E565D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2180" yWindow="500" windowWidth="35260" windowHeight="15060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -396,7 +396,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="C17" sqref="C17:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -460,7 +460,7 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:H11" si="0">G2+1</f>
+        <f t="shared" ref="H2:H7" si="0">G2+1</f>
         <v>1</v>
       </c>
       <c r="I2" s="1" t="s">

</xml_diff>